<commit_message>
commit combobox and paging and export
</commit_message>
<xml_diff>
--- a/MISA.AMIS.BE/MISA.AMIS/MISA.AMIS.Api/wwwroot/Danh_sach_nhan_vien.xlsx
+++ b/MISA.AMIS.BE/MISA.AMIS/MISA.AMIS.Api/wwwroot/Danh_sach_nhan_vien.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="191">
   <si>
     <t>DANH SÁCH NHÂN VIÊN</t>
   </si>
@@ -44,25 +44,34 @@
     <t>Tên ngân hàng</t>
   </si>
   <si>
+    <t>NV-9978</t>
+  </si>
+  <si>
+    <t>Lê Quý Nhật sửa 1</t>
+  </si>
+  <si>
+    <t>Không xác định</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thực tập sinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phòng kế toán </t>
+  </si>
+  <si>
+    <t>8709971</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ACB Bank</t>
+  </si>
+  <si>
     <t>NV-9977</t>
   </si>
   <si>
     <t>Lê Quý Nhật sửa lần thứ ba</t>
   </si>
   <si>
-    <t>Không xác định</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thực tập sinh</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Phòng kỹ thuật </t>
-  </si>
-  <si>
-    <t>8709971</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ACB Bank</t>
   </si>
   <si>
     <t>NV-9974</t>
@@ -195,9 +204,6 @@
     <t xml:space="preserve">Nguyễn Thái Trường </t>
   </si>
   <si>
-    <t xml:space="preserve"> Phòng kế toán </t>
-  </si>
-  <si>
     <t>8823251</t>
   </si>
   <si>
@@ -528,22 +534,49 @@
     <t>0938660</t>
   </si>
   <si>
+    <t>NV-5215</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>3472254</t>
+  </si>
+  <si>
     <t>NV-6922</t>
   </si>
   <si>
     <t>Trịnh Ngọc Diễm</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>5041995</t>
   </si>
   <si>
-    <t>NV-5215</t>
-  </si>
-  <si>
-    <t>3472254</t>
+    <t>NV-1384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Tuấn Anh </t>
+  </si>
+  <si>
+    <t>7288106</t>
+  </si>
+  <si>
+    <t>NV-4057</t>
+  </si>
+  <si>
+    <t>Bùi Thị Hân</t>
+  </si>
+  <si>
+    <t>0622264</t>
+  </si>
+  <si>
+    <t>NV-6148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trân Tuấn Trường </t>
+  </si>
+  <si>
+    <t>0595747</t>
   </si>
   <si>
     <t>NV-4963</t>
@@ -553,33 +586,6 @@
   </si>
   <si>
     <t>0668634</t>
-  </si>
-  <si>
-    <t>NV-6148</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trân Tuấn Trường </t>
-  </si>
-  <si>
-    <t>0595747</t>
-  </si>
-  <si>
-    <t>NV-1384</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Tuấn Anh </t>
-  </si>
-  <si>
-    <t>7288106</t>
-  </si>
-  <si>
-    <t>NV-4057</t>
-  </si>
-  <si>
-    <t>Bùi Thị Hân</t>
-  </si>
-  <si>
-    <t>0622264</t>
   </si>
 </sst>
 </file>
@@ -665,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -780,22 +786,22 @@
         <v>18</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5">
+        <v>36664</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5">
-        <v>36472</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" s="3" customFormat="1">
@@ -803,28 +809,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5">
+        <v>36472</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="G6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="5">
-        <v>36664</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="I6" s="6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1">
@@ -832,10 +838,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>12</v>
@@ -847,7 +853,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>15</v>
@@ -870,19 +876,19 @@
         <v>12</v>
       </c>
       <c r="E8" s="5">
-        <v>21779</v>
+        <v>36664</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" s="3" customFormat="1">
@@ -890,28 +896,28 @@
         <v>6</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5">
-        <v>20467</v>
+        <v>21779</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1">
@@ -919,22 +925,22 @@
         <v>7</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5">
+        <v>20467</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="5">
-        <v>28793</v>
-      </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>40</v>
@@ -954,22 +960,22 @@
         <v>42</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E11" s="5">
-        <v>28179</v>
+        <v>28793</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="I11" s="6" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1">
@@ -977,28 +983,28 @@
         <v>9</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="5">
+        <v>28179</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="G12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="5">
-        <v>23069</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="I12" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1">
@@ -1006,28 +1012,28 @@
         <v>10</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="5">
+        <v>23069</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="5">
-        <v>27220</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="1">
@@ -1035,28 +1041,28 @@
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="5">
+        <v>27220</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="5">
-        <v>36809</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="I14" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1">
@@ -1070,22 +1076,22 @@
         <v>59</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E15" s="5">
-        <v>24431</v>
+        <v>36809</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="I15" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" s="3" customFormat="1">
@@ -1093,28 +1099,28 @@
         <v>13</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="5">
+        <v>24431</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>64</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="5">
-        <v>24427</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" s="3" customFormat="1">
@@ -1122,28 +1128,28 @@
         <v>14</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5">
+        <v>24427</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="G17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="5">
-        <v>21882</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="I17" s="6" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1">
@@ -1151,28 +1157,28 @@
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="5">
+        <v>21882</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="5">
-        <v>25479</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>72</v>
-      </c>
       <c r="I18" s="6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="1">
@@ -1180,28 +1186,28 @@
         <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5">
+        <v>25479</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="5">
-        <v>29639</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>75</v>
-      </c>
       <c r="I19" s="6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" s="3" customFormat="1">
@@ -1209,28 +1215,28 @@
         <v>17</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="5">
+        <v>29639</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="5">
-        <v>21070</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>78</v>
-      </c>
       <c r="I20" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="1">
@@ -1238,28 +1244,28 @@
         <v>18</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5">
+        <v>21070</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="5">
-        <v>35488</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="I21" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1">
@@ -1267,28 +1273,28 @@
         <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="5">
+        <v>35488</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="5">
-        <v>22346</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="I22" s="6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1">
@@ -1296,28 +1302,28 @@
         <v>20</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="5">
+        <v>22346</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="5">
-        <v>28871</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>87</v>
-      </c>
       <c r="I23" s="6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1">
@@ -1325,28 +1331,28 @@
         <v>21</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="5">
+        <v>28871</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="5">
-        <v>36448</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="I24" s="6" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1">
@@ -1354,28 +1360,28 @@
         <v>22</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="D25" s="6" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="E25" s="5">
-        <v>35961</v>
+        <v>36448</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" s="3" customFormat="1">
@@ -1383,28 +1389,28 @@
         <v>23</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E26" s="5">
-        <v>24362</v>
+        <v>35961</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" s="3" customFormat="1">
@@ -1412,28 +1418,28 @@
         <v>24</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="5">
+        <v>24362</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="5">
-        <v>20826</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="I27" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" s="3" customFormat="1">
@@ -1441,28 +1447,28 @@
         <v>25</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="5">
+        <v>20826</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="5">
-        <v>28796</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>102</v>
-      </c>
       <c r="I28" s="6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" s="3" customFormat="1">
@@ -1470,28 +1476,28 @@
         <v>26</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="5">
+        <v>28796</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="5">
-        <v>34005</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="I29" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" s="3" customFormat="1">
@@ -1499,28 +1505,28 @@
         <v>27</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" s="5">
+        <v>34005</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="5">
-        <v>24441</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="I30" s="6" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" s="3" customFormat="1">
@@ -1528,28 +1534,28 @@
         <v>28</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="5">
+        <v>24441</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="5">
-        <v>26365</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="I31" s="6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1">
@@ -1557,28 +1563,28 @@
         <v>29</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="D32" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="5">
+        <v>26365</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="5">
-        <v>33356</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>114</v>
-      </c>
       <c r="I32" s="6" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1">
@@ -1586,28 +1592,28 @@
         <v>30</v>
       </c>
       <c r="B33" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="D33" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="5">
+        <v>33356</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="5">
-        <v>20190</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>117</v>
-      </c>
       <c r="I33" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" s="3" customFormat="1">
@@ -1615,28 +1621,28 @@
         <v>31</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="D34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="5">
+        <v>20190</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" s="5">
-        <v>32696</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="I34" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" s="3" customFormat="1">
@@ -1644,28 +1650,28 @@
         <v>32</v>
       </c>
       <c r="B35" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="D35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="5">
+        <v>32696</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D35" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E35" s="5">
-        <v>32465</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>123</v>
-      </c>
       <c r="I35" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" s="3" customFormat="1">
@@ -1673,28 +1679,28 @@
         <v>33</v>
       </c>
       <c r="B36" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>125</v>
-      </c>
       <c r="D36" s="6" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E36" s="5">
-        <v>33150</v>
+        <v>32465</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" s="3" customFormat="1">
@@ -1702,28 +1708,28 @@
         <v>34</v>
       </c>
       <c r="B37" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="5">
+        <v>33150</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="5">
-        <v>36788</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>129</v>
-      </c>
       <c r="I37" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" s="3" customFormat="1">
@@ -1731,28 +1737,28 @@
         <v>35</v>
       </c>
       <c r="B38" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="D38" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="5">
+        <v>36788</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E38" s="5">
-        <v>31273</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="I38" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" s="3" customFormat="1">
@@ -1760,28 +1766,28 @@
         <v>36</v>
       </c>
       <c r="B39" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="D39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="5">
+        <v>31273</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D39" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" s="5">
-        <v>36664</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="I39" s="6" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" s="3" customFormat="1">
@@ -1804,7 +1810,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>15</v>
@@ -1827,19 +1833,19 @@
         <v>12</v>
       </c>
       <c r="E41" s="5">
-        <v>26205</v>
+        <v>36664</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>139</v>
+        <v>15</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" s="3" customFormat="1">
@@ -1847,28 +1853,28 @@
         <v>39</v>
       </c>
       <c r="B42" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D42" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E42" s="5">
-        <v>23701</v>
+        <v>26205</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>141</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" s="3" customFormat="1">
@@ -1879,25 +1885,25 @@
         <v>142</v>
       </c>
       <c r="C43" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" s="5">
+        <v>23701</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43" s="5">
-        <v>29454</v>
-      </c>
-      <c r="F43" s="6" t="s">
+      <c r="I43" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="44" s="3" customFormat="1">
@@ -1905,28 +1911,28 @@
         <v>41</v>
       </c>
       <c r="B44" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="D44" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="5">
+        <v>29454</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H44" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="5">
-        <v>30481</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>147</v>
-      </c>
       <c r="I44" s="6" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" s="3" customFormat="1">
@@ -1934,28 +1940,28 @@
         <v>42</v>
       </c>
       <c r="B45" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>146</v>
-      </c>
       <c r="D45" s="6" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="E45" s="5">
-        <v>23391</v>
+        <v>30481</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>149</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" s="3" customFormat="1">
@@ -1966,25 +1972,25 @@
         <v>150</v>
       </c>
       <c r="C46" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" s="5">
+        <v>23391</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="D46" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E46" s="5">
-        <v>22260</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>152</v>
-      </c>
       <c r="I46" s="6" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" s="3" customFormat="1">
@@ -1992,28 +1998,28 @@
         <v>44</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="D47" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="5">
+        <v>22260</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H47" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" s="5">
-        <v>19525</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="I47" s="6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" s="3" customFormat="1">
@@ -2021,28 +2027,28 @@
         <v>45</v>
       </c>
       <c r="B48" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="D48" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" s="5">
+        <v>19525</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="5">
-        <v>19496</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>158</v>
-      </c>
       <c r="I48" s="6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="1">
@@ -2050,28 +2056,28 @@
         <v>46</v>
       </c>
       <c r="B49" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>160</v>
-      </c>
       <c r="D49" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E49" s="5">
-        <v>18690</v>
+        <v>19496</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" s="3" customFormat="1">
@@ -2079,28 +2085,28 @@
         <v>47</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="D50" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="5">
+        <v>18690</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" s="5">
-        <v>18640</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>164</v>
-      </c>
       <c r="I50" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" s="3" customFormat="1">
@@ -2108,28 +2114,28 @@
         <v>48</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="D51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="5">
+        <v>18640</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="5">
-        <v>18635</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>167</v>
-      </c>
       <c r="I51" s="6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" s="3" customFormat="1">
@@ -2137,28 +2143,28 @@
         <v>49</v>
       </c>
       <c r="B52" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C52" s="6" t="s">
-        <v>169</v>
-      </c>
       <c r="D52" s="6" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E52" s="5">
         <v>18635</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" s="3" customFormat="1">
@@ -2166,44 +2172,50 @@
         <v>50</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>172</v>
-      </c>
       <c r="D53" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E53" s="5"/>
-      <c r="F53" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="E53" s="5">
+        <v>18635</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="G53" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="I53" s="6"/>
+        <v>172</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="54" s="3" customFormat="1">
       <c r="A54" s="5">
         <v>51</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="6"/>
       <c r="G54" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I54" s="6"/>
     </row>
@@ -2212,21 +2224,21 @@
         <v>52</v>
       </c>
       <c r="B55" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C55" s="6" t="s">
-        <v>178</v>
-      </c>
       <c r="D55" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="6"/>
       <c r="G55" s="6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I55" s="6"/>
     </row>
@@ -2235,21 +2247,21 @@
         <v>53</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>181</v>
-      </c>
       <c r="D56" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I56" s="6"/>
     </row>
@@ -2258,21 +2270,21 @@
         <v>54</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="C57" s="6" t="s">
-        <v>184</v>
-      </c>
       <c r="D57" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="6"/>
       <c r="G57" s="6" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I57" s="6"/>
     </row>
@@ -2281,23 +2293,46 @@
         <v>55</v>
       </c>
       <c r="B58" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>187</v>
-      </c>
       <c r="D58" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="6"/>
       <c r="G58" s="6" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="H58" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" s="3" customFormat="1">
+      <c r="A59" s="5">
+        <v>56</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="I58" s="6"/>
+      <c r="C59" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="I59" s="6"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>